<commit_message>
ajout mode api et ihm
</commit_message>
<xml_diff>
--- a/rapport/rapport_api.xlsx
+++ b/rapport/rapport_api.xlsx
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>3.677576781577338</v>
+        <v>3.677627633308154</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>57.9856687770389</v>
+        <v>57.96693520079926</v>
       </c>
     </row>
     <row r="3">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>3.150988480125088</v>
+        <v>3.151019696039055</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>7.238477791174596</v>
+        <v>7.238308117577713</v>
       </c>
     </row>
     <row r="4">
@@ -512,7 +512,7 @@
         <v>71</v>
       </c>
       <c r="C4" t="n">
-        <v>0.264617302692309</v>
+        <v>0.2646268688594923</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>5.740059796425328</v>
+        <v>5.740000133751053</v>
       </c>
     </row>
     <row r="5">
@@ -533,7 +533,7 @@
         <v>71</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2619709987599403</v>
+        <v>0.2619810684096068</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>5.498332821355016</v>
+        <v>5.498352708913107</v>
       </c>
     </row>
     <row r="6">
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>7.160235858041793</v>
+        <v>7.160682698745746</v>
       </c>
     </row>
     <row r="7">
@@ -566,7 +566,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>7.160264556543343</v>
+        <v>7.160431964469049</v>
       </c>
     </row>
     <row r="8">
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>7.17010562516246</v>
+        <v>7.160410566463508</v>
       </c>
     </row>
     <row r="9">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>7.170182406241167</v>
+        <v>7.170478957423848</v>
       </c>
     </row>
     <row r="10">
@@ -625,7 +625,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>2.007661072909646</v>
+        <v>2.007575984369963</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -633,7 +633,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>7.170433140517865</v>
+        <v>7.16064242014708</v>
       </c>
     </row>
     <row r="11">
@@ -646,7 +646,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>2.079797022225895</v>
+        <v>2.079712437168695</v>
       </c>
     </row>
     <row r="13">
@@ -683,7 +683,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>3.151041094044596</v>
+        <v>3.150995277138613</v>
       </c>
     </row>
     <row r="16">
@@ -696,7 +696,7 @@
         <v>9</v>
       </c>
       <c r="C16" t="n">
-        <v>2.272232558695972</v>
+        <v>2.272233565660938</v>
       </c>
     </row>
     <row r="17">
@@ -709,7 +709,7 @@
         <v>65</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3167861436847598</v>
+        <v>0.3167712909515016</v>
       </c>
     </row>
     <row r="19">
@@ -746,7 +746,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>3.151019696039055</v>
+        <v>3.151041094044596</v>
       </c>
     </row>
     <row r="22">
@@ -772,7 +772,7 @@
         <v>63</v>
       </c>
       <c r="C23" t="n">
-        <v>0.3474666040300392</v>
+        <v>0.3474650935825892</v>
       </c>
     </row>
     <row r="25">
@@ -809,7 +809,7 @@
         <v>6</v>
       </c>
       <c r="C27" t="n">
-        <v>3.151019696039055</v>
+        <v>3.150995277138613</v>
       </c>
     </row>
     <row r="28">
@@ -822,7 +822,7 @@
         <v>14</v>
       </c>
       <c r="C28" t="n">
-        <v>1.682378410577495</v>
+        <v>1.682770875173248</v>
       </c>
     </row>
     <row r="29">
@@ -835,7 +835,7 @@
         <v>9</v>
       </c>
       <c r="C29" t="n">
-        <v>2.326837751425244</v>
+        <v>2.326916546433885</v>
       </c>
     </row>
     <row r="31">
@@ -872,7 +872,7 @@
         <v>6</v>
       </c>
       <c r="C33" t="n">
-        <v>3.150995277138613</v>
+        <v>3.151041094044596</v>
       </c>
     </row>
     <row r="34">
@@ -885,7 +885,7 @@
         <v>14</v>
       </c>
       <c r="C34" t="n">
-        <v>1.682397542911861</v>
+        <v>1.682474323990569</v>
       </c>
     </row>
     <row r="35">
@@ -898,7 +898,7 @@
         <v>9</v>
       </c>
       <c r="C35" t="n">
-        <v>2.326871736492869</v>
+        <v>2.326916546433885</v>
       </c>
     </row>
     <row r="37">
@@ -935,7 +935,7 @@
         <v>6</v>
       </c>
       <c r="C39" t="n">
-        <v>3.151041094044596</v>
+        <v>3.151019696039055</v>
       </c>
     </row>
     <row r="40">
@@ -948,7 +948,7 @@
         <v>14</v>
       </c>
       <c r="C40" t="n">
-        <v>1.682397542911861</v>
+        <v>1.682474323990569</v>
       </c>
     </row>
     <row r="41">
@@ -961,7 +961,7 @@
         <v>9</v>
       </c>
       <c r="C41" t="n">
-        <v>2.336666988206003</v>
+        <v>2.326916546433885</v>
       </c>
     </row>
     <row r="43">
@@ -1011,7 +1011,7 @@
         <v>14</v>
       </c>
       <c r="C46" t="n">
-        <v>1.682474323990569</v>
+        <v>1.682770875173248</v>
       </c>
     </row>
     <row r="47">
@@ -1061,7 +1061,7 @@
         <v>6</v>
       </c>
       <c r="C51" t="n">
-        <v>3.150995277138613</v>
+        <v>3.151019696039055</v>
       </c>
     </row>
     <row r="52">
@@ -1074,7 +1074,7 @@
         <v>14</v>
       </c>
       <c r="C52" t="n">
-        <v>1.682770875173248</v>
+        <v>1.682474323990569</v>
       </c>
     </row>
     <row r="53">
@@ -1087,7 +1087,7 @@
         <v>9</v>
       </c>
       <c r="C53" t="n">
-        <v>2.336666988206003</v>
+        <v>2.327148400117457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>